<commit_message>
update to template v2
</commit_message>
<xml_diff>
--- a/inst/templates/mdJSONdictio_Dictionary_Template_v2.xlsx
+++ b/inst/templates/mdJSONdictio_Dictionary_Template_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/hannah_vincelette_fws_gov/Documents/Documents/GitHub/mdJSONdictio/inst/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="11_365F113B0B881ECF37D0853E5545BA4ACE1F468E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C959183-A050-4246-894B-F250F83DA1F6}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="11_365F113B0B881ECF37D0853E5545BA4ACE1F468E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{602A727C-69D9-495E-8BCC-6A284ACFB677}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="3915" windowWidth="25170" windowHeight="8520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_dictionary" sheetId="1" r:id="rId1"/>
@@ -707,26 +707,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -816,26 +817,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.85546875" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1993,21 +1995,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DE904D578DFE6844BEAE84BDC2B4097E" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5270cfe5b55ea3ba0621c55bb260cb69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="847bd2b6-c417-48b3-84b7-e392c504f3bb" xmlns:ns4="f32a61f4-5698-46d5-9f56-343e6d7dc7d7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2f6d81c817a7b765436e9b6c5a88d8e2" ns3:_="" ns4:_="">
     <xsd:import namespace="847bd2b6-c417-48b3-84b7-e392c504f3bb"/>
@@ -2222,32 +2209,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A7F80B6-A8F8-4FBE-8961-7EA21E322D52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f32a61f4-5698-46d5-9f56-343e6d7dc7d7"/>
-    <ds:schemaRef ds:uri="847bd2b6-c417-48b3-84b7-e392c504f3bb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAD0FC99-4A9C-4418-97BD-C5AA74E03F40}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA5209D-AC5E-47D6-BDE1-DC1FA12E6F85}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2264,4 +2241,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAD0FC99-4A9C-4418-97BD-C5AA74E03F40}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A7F80B6-A8F8-4FBE-8961-7EA21E322D52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f32a61f4-5698-46d5-9f56-343e6d7dc7d7"/>
+    <ds:schemaRef ds:uri="847bd2b6-c417-48b3-84b7-e392c504f3bb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>